<commit_message>
improved the cross validation activity which is used for validation
</commit_message>
<xml_diff>
--- a/Cross-Validation SVM/SupportVextors/ResultMat/ResultMat4Users.xlsx
+++ b/Cross-Validation SVM/SupportVextors/ResultMat/ResultMat4Users.xlsx
@@ -846,7 +846,7 @@
   <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2681,11 +2681,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="N1:O88">
-    <sortState ref="N2:O88">
-      <sortCondition ref="N1:N88"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>